<commit_message>
This will finish the Package excel mapping and add the finished excel mapping for the Customer. I have also added all my PDF's in a landscape format to make it easier to view via an internet browser.
</commit_message>
<xml_diff>
--- a/Team_02_M2_Final_Submission/Team_02_M2_D1_Dimension_Mapping_metadata/support/Team_02_M2_D1_Dimension_Mapping_Dealer.xlsx
+++ b/Team_02_M2_Final_Submission/Team_02_M2_D1_Dimension_Mapping_metadata/support/Team_02_M2_D1_Dimension_Mapping_Dealer.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\M2\work\Team_02_M2_Final_Submission\Team_02_M2_D1_Dimension_Mapping_metadata\support\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{157D53E9-12A4-43A7-B76C-9110D572C10C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23B40DF0-F012-4C9B-A710-D2DD58520716}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="660" yWindow="1875" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6975" yWindow="2310" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dealer" sheetId="1" r:id="rId1"/>
@@ -660,7 +660,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
@@ -1264,7 +1264,7 @@
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
This updates the Mapping of my dealer spreadsheet and the pdf in order to better align with the sources so that when we go to do our ETL portion of the project, we can then have the ease of being able to bring in chunks of infomration in batches from one source instead of multiple.
</commit_message>
<xml_diff>
--- a/Team_02_M2_Final_Submission/Team_02_M2_D1_Dimension_Mapping_metadata/support/Team_02_M2_D1_Dimension_Mapping_Dealer.xlsx
+++ b/Team_02_M2_Final_Submission/Team_02_M2_D1_Dimension_Mapping_metadata/support/Team_02_M2_D1_Dimension_Mapping_Dealer.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\M2\work\Team_02_M2_Final_Submission\Team_02_M2_D1_Dimension_Mapping_metadata\support\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23B40DF0-F012-4C9B-A710-D2DD58520716}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79F93ADF-8E7B-4619-B1A0-DBD40DCDDD46}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6975" yWindow="2310" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dealer" sheetId="1" r:id="rId1"/>
@@ -661,7 +661,7 @@
   <dimension ref="A1:L20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -773,19 +773,19 @@
         <v>12</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="F4" s="11" t="s">
         <v>12</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="I4" s="16" t="s">
         <v>12</v>
@@ -987,22 +987,22 @@
         <v>19</v>
       </c>
       <c r="D11" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="G11" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="E11" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="F11" s="9" t="s">
+      <c r="H11" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="I11" s="9" t="s">
         <v>19</v>
-      </c>
-      <c r="G11" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="H11" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="I11" s="9" t="s">
-        <v>40</v>
       </c>
       <c r="J11" s="9" t="s">
         <v>9</v>
@@ -1129,22 +1129,22 @@
         <v>24</v>
       </c>
       <c r="D16" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G16" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="E16" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F16" s="2" t="s">
+      <c r="H16" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="I16" s="6" t="s">
         <v>44</v>
-      </c>
-      <c r="G16" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="H16" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="I16" s="6" t="s">
-        <v>45</v>
       </c>
       <c r="J16" s="8"/>
       <c r="K16" s="8"/>

</xml_diff>

<commit_message>
Updates to the Package and Dealer excel files which have now been updated to assist in the mapping for our ETL. Also deleted the previous ETL files sent by Hytham after speaking to the Professor.
</commit_message>
<xml_diff>
--- a/Team_02_M2_Final_Submission/Team_02_M2_D1_Dimension_Mapping_metadata/support/Team_02_M2_D1_Dimension_Mapping_Dealer.xlsx
+++ b/Team_02_M2_Final_Submission/Team_02_M2_D1_Dimension_Mapping_metadata/support/Team_02_M2_D1_Dimension_Mapping_Dealer.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\M2\work\Team_02_M2_Final_Submission\Team_02_M2_D1_Dimension_Mapping_metadata\support\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79F93ADF-8E7B-4619-B1A0-DBD40DCDDD46}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CAFFA70-5C8F-401B-948B-D1D1B908F87A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3315" yWindow="6780" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dealer" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="51">
   <si>
     <t>Database</t>
   </si>
@@ -127,24 +127,12 @@
     <t>Branch</t>
   </si>
   <si>
-    <t>BR_Address</t>
-  </si>
-  <si>
-    <t>BR_City</t>
-  </si>
-  <si>
     <t>BR_Country</t>
   </si>
   <si>
     <t>BR_County</t>
   </si>
   <si>
-    <t>BR_State</t>
-  </si>
-  <si>
-    <t>BR_Zip</t>
-  </si>
-  <si>
     <t>DLR_Type</t>
   </si>
   <si>
@@ -173,6 +161,18 @@
   </si>
   <si>
     <t>WEB_Start_Date</t>
+  </si>
+  <si>
+    <t>ID_Name</t>
+  </si>
+  <si>
+    <t>Owner_Address</t>
+  </si>
+  <si>
+    <t>OADR_County</t>
+  </si>
+  <si>
+    <t>OADR_Country</t>
   </si>
 </sst>
 </file>
@@ -661,7 +661,7 @@
   <dimension ref="A1:L20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:C1"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -673,8 +673,8 @@
     <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="26.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="25.85546875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="6.28515625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="9.85546875" bestFit="1" customWidth="1"/>
@@ -773,32 +773,20 @@
         <v>12</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>31</v>
+        <v>9</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="F4" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="G4" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="H4" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="I4" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="J4" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="K4" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="L4" s="8" t="s">
-        <v>12</v>
-      </c>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="16"/>
+      <c r="J4" s="17"/>
+      <c r="K4" s="8"/>
+      <c r="L4" s="8"/>
     </row>
     <row r="5" spans="1:12" s="10" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
@@ -819,9 +807,15 @@
       <c r="F5" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="9"/>
+      <c r="G5" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="H5" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="I5" s="9" t="s">
+        <v>47</v>
+      </c>
       <c r="J5" s="9"/>
       <c r="K5" s="9"/>
       <c r="L5" s="9"/>
@@ -837,23 +831,17 @@
         <v>14</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>31</v>
+        <v>9</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>34</v>
+        <v>10</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="G6" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="H6" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="I6" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
       <c r="J6" s="8"/>
       <c r="K6" s="8"/>
       <c r="L6" s="8"/>
@@ -869,23 +857,17 @@
         <v>15</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>31</v>
+        <v>9</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>34</v>
+        <v>10</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="G7" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="H7" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="I7" s="9" t="s">
         <v>15</v>
       </c>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
       <c r="J7" s="9"/>
       <c r="K7" s="9"/>
       <c r="L7" s="9"/>
@@ -907,13 +889,17 @@
         <v>34</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="H8" s="6"/>
-      <c r="I8" s="6"/>
+        <v>31</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="I8" s="6" t="s">
+        <v>49</v>
+      </c>
       <c r="J8" s="8"/>
       <c r="K8" s="8"/>
       <c r="L8" s="8"/>
@@ -929,23 +915,17 @@
         <v>17</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>31</v>
+        <v>9</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>34</v>
+        <v>10</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="G9" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="H9" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="I9" s="9" t="s">
         <v>17</v>
       </c>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
       <c r="J9" s="9"/>
       <c r="K9" s="9"/>
       <c r="L9" s="9"/>
@@ -967,11 +947,17 @@
         <v>34</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="6"/>
+        <v>35</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="I10" s="6" t="s">
+        <v>50</v>
+      </c>
       <c r="J10" s="8"/>
       <c r="K10" s="8"/>
       <c r="L10" s="8"/>
@@ -987,32 +973,20 @@
         <v>19</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>31</v>
+        <v>9</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>34</v>
+        <v>10</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="G11" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="H11" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="I11" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="J11" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="K11" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="L11" s="9" t="s">
-        <v>19</v>
-      </c>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="9"/>
+      <c r="K11" s="9"/>
+      <c r="L11" s="9"/>
     </row>
     <row r="12" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
@@ -1031,7 +1005,7 @@
         <v>10</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="G12" s="6"/>
       <c r="H12" s="6"/>
@@ -1057,7 +1031,7 @@
         <v>30</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="G13" s="9"/>
       <c r="H13" s="9"/>
@@ -1083,7 +1057,7 @@
         <v>30</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="G14" s="6"/>
       <c r="H14" s="6"/>
@@ -1109,7 +1083,7 @@
         <v>30</v>
       </c>
       <c r="F15" s="9" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="G15" s="9"/>
       <c r="H15" s="9"/>
@@ -1135,7 +1109,7 @@
         <v>34</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="G16" s="6" t="s">
         <v>29</v>
@@ -1144,7 +1118,7 @@
         <v>10</v>
       </c>
       <c r="I16" s="6" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="J16" s="8"/>
       <c r="K16" s="8"/>
@@ -1164,10 +1138,10 @@
         <v>31</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="F17" s="9" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="G17" s="9"/>
       <c r="H17" s="9"/>
@@ -1190,10 +1164,10 @@
         <v>31</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="G18" s="6"/>
       <c r="H18" s="6"/>
@@ -1216,10 +1190,10 @@
         <v>31</v>
       </c>
       <c r="E19" s="9" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="F19" s="9" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="G19" s="9"/>
       <c r="H19" s="9"/>
@@ -1242,10 +1216,10 @@
         <v>31</v>
       </c>
       <c r="E20" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F20" s="2" t="s">
         <v>46</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>50</v>
       </c>
       <c r="G20" s="6"/>
       <c r="H20" s="6"/>

</xml_diff>

<commit_message>
Final review of the Mapping for Dealer. Did more domain studies which showed me that less sources were needed on multiple columns.
</commit_message>
<xml_diff>
--- a/Team_02_M2_Final_Submission/Team_02_M2_D1_Dimension_Mapping_metadata/support/Team_02_M2_D1_Dimension_Mapping_Dealer.xlsx
+++ b/Team_02_M2_Final_Submission/Team_02_M2_D1_Dimension_Mapping_metadata/support/Team_02_M2_D1_Dimension_Mapping_Dealer.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\M2\work\Team_02_M2_Final_Submission\Team_02_M2_D1_Dimension_Mapping_metadata\support\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CAFFA70-5C8F-401B-948B-D1D1B908F87A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DCC721A-2A02-4A21-A1A2-085DD5FB99A8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3315" yWindow="6780" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3735" yWindow="4215" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dealer" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="47">
   <si>
     <t>Database</t>
   </si>
@@ -145,9 +145,6 @@
     <t>DLR_Phone</t>
   </si>
   <si>
-    <t>BR_Phone</t>
-  </si>
-  <si>
     <t>Website</t>
   </si>
   <si>
@@ -164,15 +161,6 @@
   </si>
   <si>
     <t>ID_Name</t>
-  </si>
-  <si>
-    <t>Owner_Address</t>
-  </si>
-  <si>
-    <t>OADR_County</t>
-  </si>
-  <si>
-    <t>OADR_Country</t>
   </si>
 </sst>
 </file>
@@ -661,7 +649,7 @@
   <dimension ref="A1:L20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="G8" sqref="G8:I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -814,7 +802,7 @@
         <v>30</v>
       </c>
       <c r="I5" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J5" s="9"/>
       <c r="K5" s="9"/>
@@ -891,15 +879,9 @@
       <c r="F8" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="G8" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="H8" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="I8" s="6" t="s">
-        <v>49</v>
-      </c>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
       <c r="J8" s="8"/>
       <c r="K8" s="8"/>
       <c r="L8" s="8"/>
@@ -949,15 +931,9 @@
       <c r="F10" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="G10" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="H10" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="I10" s="6" t="s">
-        <v>50</v>
-      </c>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
       <c r="J10" s="8"/>
       <c r="K10" s="8"/>
       <c r="L10" s="8"/>
@@ -1103,23 +1079,17 @@
         <v>24</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>34</v>
+        <v>10</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="G16" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="H16" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="I16" s="6" t="s">
         <v>40</v>
       </c>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
       <c r="J16" s="8"/>
       <c r="K16" s="8"/>
       <c r="L16" s="8"/>
@@ -1138,10 +1108,10 @@
         <v>31</v>
       </c>
       <c r="E17" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="F17" s="9" t="s">
         <v>42</v>
-      </c>
-      <c r="F17" s="9" t="s">
-        <v>43</v>
       </c>
       <c r="G17" s="9"/>
       <c r="H17" s="9"/>
@@ -1164,10 +1134,10 @@
         <v>31</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G18" s="6"/>
       <c r="H18" s="6"/>
@@ -1190,10 +1160,10 @@
         <v>31</v>
       </c>
       <c r="E19" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F19" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G19" s="9"/>
       <c r="H19" s="9"/>
@@ -1216,10 +1186,10 @@
         <v>31</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G20" s="6"/>
       <c r="H20" s="6"/>

</xml_diff>

<commit_message>
Update of the mapping for Dealer to include the Owner Address for County and Country. This way the join would allow us to see all of the things we needed for this. As well, all the SQL files through the Insertion of data into our Staged table will allow us to start building our package.
</commit_message>
<xml_diff>
--- a/Team_02_M2_Final_Submission/Team_02_M2_D1_Dimension_Mapping_metadata/support/Team_02_M2_D1_Dimension_Mapping_Dealer.xlsx
+++ b/Team_02_M2_Final_Submission/Team_02_M2_D1_Dimension_Mapping_metadata/support/Team_02_M2_D1_Dimension_Mapping_Dealer.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\M2\work\Team_02_M2_Final_Submission\Team_02_M2_D1_Dimension_Mapping_metadata\support\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DCC721A-2A02-4A21-A1A2-085DD5FB99A8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F744DA11-7B88-446D-A07D-9707C1E6BC08}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3735" yWindow="4215" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="50">
   <si>
     <t>Database</t>
   </si>
@@ -161,6 +161,15 @@
   </si>
   <si>
     <t>ID_Name</t>
+  </si>
+  <si>
+    <t>Owner_Address</t>
+  </si>
+  <si>
+    <t>OADR_County</t>
+  </si>
+  <si>
+    <t>OADR_Country</t>
   </si>
 </sst>
 </file>
@@ -649,7 +658,7 @@
   <dimension ref="A1:L20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8:I8"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -879,9 +888,15 @@
       <c r="F8" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="6"/>
+      <c r="G8" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="I8" s="6" t="s">
+        <v>48</v>
+      </c>
       <c r="J8" s="8"/>
       <c r="K8" s="8"/>
       <c r="L8" s="8"/>
@@ -931,9 +946,15 @@
       <c r="F10" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="6"/>
+      <c r="G10" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="I10" s="6" t="s">
+        <v>49</v>
+      </c>
       <c r="J10" s="8"/>
       <c r="K10" s="8"/>
       <c r="L10" s="8"/>

</xml_diff>